<commit_message>
corrected VAR labeling errors in spelling
</commit_message>
<xml_diff>
--- a/BLS_Hourly_Wage/Warehouse_BLS.xlsx
+++ b/BLS_Hourly_Wage/Warehouse_BLS.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,35 +456,45 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>General warehousing and storage - Under 16 years</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>General warehousing and storage - 16 to 17 years</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>General warehousing and storage - 18 to 19 years</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>General warehousing and storage - 20 to 24 years</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>General warehousing and storage - 25 to 34 years</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>General warehousing and storage - 35 to 44 years</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>General warehousing and storage - 45 to 54 years</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>General warehousing and storage - 55 to 64 years</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>General warehousing and storage - 65 years and over</t>
         </is>
@@ -503,25 +513,35 @@
       <c r="D2" t="n">
         <v>36</v>
       </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0</v>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" t="n">
         <v>10</v>
       </c>
-      <c r="H2" t="n">
+      <c r="J2" t="n">
         <v>6</v>
       </c>
-      <c r="I2" t="n">
+      <c r="K2" t="n">
         <v>9</v>
       </c>
-      <c r="J2" t="n">
+      <c r="L2" t="n">
         <v>7</v>
       </c>
-      <c r="K2" t="n">
+      <c r="M2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -538,25 +558,35 @@
       <c r="D3" t="n">
         <v>11</v>
       </c>
-      <c r="E3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" t="n">
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
         <v>1</v>
       </c>
-      <c r="G3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0</v>
-      </c>
       <c r="I3" t="n">
         <v>0</v>
       </c>
       <c r="J3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" t="n">
         <v>3</v>
       </c>
-      <c r="K3" t="n">
+      <c r="M3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -573,11 +603,15 @@
       <c r="D4" t="n">
         <v>17</v>
       </c>
-      <c r="E4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0</v>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="G4" t="n">
         <v>0</v>
@@ -586,12 +620,18 @@
         <v>0</v>
       </c>
       <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" t="n">
         <v>4</v>
       </c>
-      <c r="J4" t="n">
+      <c r="L4" t="n">
         <v>5</v>
       </c>
-      <c r="K4" t="n">
+      <c r="M4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -608,25 +648,35 @@
       <c r="D5" t="n">
         <v>13</v>
       </c>
-      <c r="E5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0</v>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
         <v>4</v>
       </c>
-      <c r="H5" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" t="n">
-        <v>0</v>
-      </c>
       <c r="J5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" t="n">
         <v>3</v>
       </c>
-      <c r="K5" t="n">
+      <c r="M5" t="n">
         <v>1</v>
       </c>
     </row>
@@ -643,14 +693,18 @@
       <c r="D6" t="n">
         <v>15</v>
       </c>
-      <c r="E6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0</v>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="G6" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
@@ -662,6 +716,12 @@
         <v>0</v>
       </c>
       <c r="K6" t="n">
+        <v>4</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" t="n">
         <v>3</v>
       </c>
     </row>
@@ -678,25 +738,35 @@
       <c r="D7" t="n">
         <v>12</v>
       </c>
-      <c r="E7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" t="n">
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
         <v>1</v>
       </c>
-      <c r="G7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H7" t="n">
-        <v>0</v>
-      </c>
       <c r="I7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" t="n">
         <v>6</v>
       </c>
-      <c r="J7" t="n">
+      <c r="L7" t="n">
         <v>4</v>
       </c>
-      <c r="K7" t="n">
+      <c r="M7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -713,25 +783,35 @@
       <c r="D8" t="n">
         <v>6</v>
       </c>
-      <c r="E8" t="n">
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G8" t="n">
         <v>1</v>
       </c>
-      <c r="F8" t="n">
-        <v>0</v>
-      </c>
-      <c r="G8" t="n">
-        <v>0</v>
-      </c>
       <c r="H8" t="n">
         <v>0</v>
       </c>
       <c r="I8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" t="n">
         <v>1</v>
       </c>
-      <c r="J8" t="n">
-        <v>0</v>
-      </c>
-      <c r="K8" t="n">
+      <c r="L8" t="n">
+        <v>0</v>
+      </c>
+      <c r="M8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -748,25 +828,35 @@
       <c r="D9" t="n">
         <v>13</v>
       </c>
-      <c r="E9" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0</v>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" t="n">
         <v>3</v>
       </c>
-      <c r="H9" t="n">
+      <c r="J9" t="n">
         <v>1</v>
       </c>
-      <c r="I9" t="n">
-        <v>0</v>
-      </c>
-      <c r="J9" t="n">
-        <v>0</v>
-      </c>
       <c r="K9" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" t="n">
         <v>4</v>
       </c>
     </row>
@@ -783,25 +873,35 @@
       <c r="D10" t="n">
         <v>13</v>
       </c>
-      <c r="E10" t="n">
-        <v>0</v>
-      </c>
-      <c r="F10" t="n">
-        <v>0</v>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="G10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" t="n">
         <v>5</v>
       </c>
-      <c r="H10" t="n">
-        <v>0</v>
-      </c>
-      <c r="I10" t="n">
+      <c r="J10" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" t="n">
         <v>3</v>
       </c>
-      <c r="J10" t="n">
+      <c r="L10" t="n">
         <v>3</v>
       </c>
-      <c r="K10" t="n">
+      <c r="M10" t="n">
         <v>0</v>
       </c>
     </row>
@@ -818,11 +918,15 @@
       <c r="D11" t="n">
         <v>4</v>
       </c>
-      <c r="E11" t="n">
-        <v>0</v>
-      </c>
-      <c r="F11" t="n">
-        <v>0</v>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="G11" t="n">
         <v>0</v>
@@ -837,6 +941,12 @@
         <v>0</v>
       </c>
       <c r="K11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0</v>
+      </c>
+      <c r="M11" t="n">
         <v>0</v>
       </c>
     </row>
@@ -853,25 +963,35 @@
       <c r="D12" t="n">
         <v>7</v>
       </c>
-      <c r="E12" t="n">
-        <v>0</v>
-      </c>
-      <c r="F12" t="n">
-        <v>0</v>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="G12" t="n">
         <v>0</v>
       </c>
       <c r="H12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" t="n">
         <v>1</v>
       </c>
-      <c r="I12" t="n">
-        <v>0</v>
-      </c>
-      <c r="J12" t="n">
+      <c r="K12" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" t="n">
         <v>2</v>
       </c>
-      <c r="K12" t="n">
+      <c r="M12" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changed column created if IF to floats
</commit_message>
<xml_diff>
--- a/BLS_Hourly_Wage/Warehouse_BLS.xlsx
+++ b/BLS_Hourly_Wage/Warehouse_BLS.xlsx
@@ -513,15 +513,11 @@
       <c r="D2" t="n">
         <v>36</v>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
@@ -558,15 +554,11 @@
       <c r="D3" t="n">
         <v>11</v>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
@@ -603,15 +595,11 @@
       <c r="D4" t="n">
         <v>17</v>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
       </c>
       <c r="G4" t="n">
         <v>0</v>
@@ -648,15 +636,11 @@
       <c r="D5" t="n">
         <v>13</v>
       </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
       </c>
       <c r="G5" t="n">
         <v>0</v>
@@ -693,15 +677,11 @@
       <c r="D6" t="n">
         <v>15</v>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
       </c>
       <c r="G6" t="n">
         <v>0</v>
@@ -738,15 +718,11 @@
       <c r="D7" t="n">
         <v>12</v>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
       </c>
       <c r="G7" t="n">
         <v>0</v>
@@ -783,15 +759,11 @@
       <c r="D8" t="n">
         <v>6</v>
       </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
       </c>
       <c r="G8" t="n">
         <v>1</v>
@@ -828,15 +800,11 @@
       <c r="D9" t="n">
         <v>13</v>
       </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
       </c>
       <c r="G9" t="n">
         <v>0</v>
@@ -873,15 +841,11 @@
       <c r="D10" t="n">
         <v>13</v>
       </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="E10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0</v>
       </c>
       <c r="G10" t="n">
         <v>0</v>
@@ -918,15 +882,11 @@
       <c r="D11" t="n">
         <v>4</v>
       </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="E11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0</v>
       </c>
       <c r="G11" t="n">
         <v>0</v>
@@ -963,15 +923,11 @@
       <c r="D12" t="n">
         <v>7</v>
       </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="E12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0</v>
       </c>
       <c r="G12" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
corrected merge and export to excel WITH index
</commit_message>
<xml_diff>
--- a/BLS_Hourly_Wage/Warehouse_BLS.xlsx
+++ b/BLS_Hourly_Wage/Warehouse_BLS.xlsx
@@ -501,8 +501,10 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>2021</v>
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
       </c>
       <c r="B2" t="n">
         <v>4728</v>
@@ -513,18 +515,10 @@
       <c r="D2" t="n">
         <v>36</v>
       </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0</v>
-      </c>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
       <c r="I2" t="n">
         <v>10</v>
       </c>
@@ -537,13 +531,13 @@
       <c r="L2" t="n">
         <v>7</v>
       </c>
-      <c r="M2" t="n">
-        <v>0</v>
-      </c>
+      <c r="M2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>2020</v>
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
       </c>
       <c r="B3" t="n">
         <v>4349</v>
@@ -554,37 +548,25 @@
       <c r="D3" t="n">
         <v>11</v>
       </c>
-      <c r="E3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0</v>
-      </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
       <c r="H3" t="n">
         <v>1</v>
       </c>
-      <c r="I3" t="n">
-        <v>0</v>
-      </c>
-      <c r="J3" t="n">
-        <v>0</v>
-      </c>
-      <c r="K3" t="n">
-        <v>0</v>
-      </c>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
       <c r="L3" t="n">
         <v>3</v>
       </c>
-      <c r="M3" t="n">
-        <v>0</v>
-      </c>
+      <c r="M3" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>2019</v>
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
       </c>
       <c r="B4" t="n">
         <v>4907</v>
@@ -595,37 +577,25 @@
       <c r="D4" t="n">
         <v>17</v>
       </c>
-      <c r="E4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4" t="n">
-        <v>0</v>
-      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
       <c r="K4" t="n">
         <v>4</v>
       </c>
       <c r="L4" t="n">
         <v>5</v>
       </c>
-      <c r="M4" t="n">
-        <v>0</v>
-      </c>
+      <c r="M4" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>2018</v>
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
       </c>
       <c r="B5" t="n">
         <v>4779</v>
@@ -636,27 +606,15 @@
       <c r="D5" t="n">
         <v>13</v>
       </c>
-      <c r="E5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0</v>
-      </c>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
       <c r="I5" t="n">
         <v>4</v>
       </c>
-      <c r="J5" t="n">
-        <v>0</v>
-      </c>
-      <c r="K5" t="n">
-        <v>0</v>
-      </c>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
       <c r="L5" t="n">
         <v>3</v>
       </c>
@@ -665,8 +623,10 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>2017</v>
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>2017</t>
+        </is>
       </c>
       <c r="B6" t="n">
         <v>4674</v>
@@ -677,37 +637,27 @@
       <c r="D6" t="n">
         <v>15</v>
       </c>
-      <c r="E6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0</v>
-      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
       <c r="I6" t="n">
         <v>4</v>
       </c>
-      <c r="J6" t="n">
-        <v>0</v>
-      </c>
+      <c r="J6" t="inlineStr"/>
       <c r="K6" t="n">
         <v>4</v>
       </c>
-      <c r="L6" t="n">
-        <v>0</v>
-      </c>
+      <c r="L6" t="inlineStr"/>
       <c r="M6" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>2016</v>
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>2016</t>
+        </is>
       </c>
       <c r="B7" t="n">
         <v>4693</v>
@@ -718,37 +668,27 @@
       <c r="D7" t="n">
         <v>12</v>
       </c>
-      <c r="E7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0</v>
-      </c>
-      <c r="G7" t="n">
-        <v>0</v>
-      </c>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
       <c r="H7" t="n">
         <v>1</v>
       </c>
-      <c r="I7" t="n">
-        <v>0</v>
-      </c>
-      <c r="J7" t="n">
-        <v>0</v>
-      </c>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
       <c r="K7" t="n">
         <v>6</v>
       </c>
       <c r="L7" t="n">
         <v>4</v>
       </c>
-      <c r="M7" t="n">
-        <v>0</v>
-      </c>
+      <c r="M7" t="inlineStr"/>
     </row>
     <row r="8">
-      <c r="A8" t="n">
-        <v>2015</v>
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>2015</t>
+        </is>
       </c>
       <c r="B8" t="n">
         <v>4379</v>
@@ -759,37 +699,25 @@
       <c r="D8" t="n">
         <v>6</v>
       </c>
-      <c r="E8" t="n">
-        <v>0</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0</v>
-      </c>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
       <c r="G8" t="n">
         <v>1</v>
       </c>
-      <c r="H8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I8" t="n">
-        <v>0</v>
-      </c>
-      <c r="J8" t="n">
-        <v>0</v>
-      </c>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
       <c r="K8" t="n">
         <v>1</v>
       </c>
-      <c r="L8" t="n">
-        <v>0</v>
-      </c>
-      <c r="M8" t="n">
-        <v>0</v>
-      </c>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
     </row>
     <row r="9">
-      <c r="A9" t="n">
-        <v>2014</v>
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>2014</t>
+        </is>
       </c>
       <c r="B9" t="n">
         <v>4386</v>
@@ -800,37 +728,27 @@
       <c r="D9" t="n">
         <v>13</v>
       </c>
-      <c r="E9" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0</v>
-      </c>
-      <c r="G9" t="n">
-        <v>0</v>
-      </c>
-      <c r="H9" t="n">
-        <v>0</v>
-      </c>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
       <c r="I9" t="n">
         <v>3</v>
       </c>
       <c r="J9" t="n">
         <v>1</v>
       </c>
-      <c r="K9" t="n">
-        <v>0</v>
-      </c>
-      <c r="L9" t="n">
-        <v>0</v>
-      </c>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
       <c r="M9" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
-        <v>2013</v>
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>2013</t>
+        </is>
       </c>
       <c r="B10" t="n">
         <v>4101</v>
@@ -841,37 +759,27 @@
       <c r="D10" t="n">
         <v>13</v>
       </c>
-      <c r="E10" t="n">
-        <v>0</v>
-      </c>
-      <c r="F10" t="n">
-        <v>0</v>
-      </c>
-      <c r="G10" t="n">
-        <v>0</v>
-      </c>
-      <c r="H10" t="n">
-        <v>0</v>
-      </c>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
       <c r="I10" t="n">
         <v>5</v>
       </c>
-      <c r="J10" t="n">
-        <v>0</v>
-      </c>
+      <c r="J10" t="inlineStr"/>
       <c r="K10" t="n">
         <v>3</v>
       </c>
       <c r="L10" t="n">
         <v>3</v>
       </c>
-      <c r="M10" t="n">
-        <v>0</v>
-      </c>
+      <c r="M10" t="inlineStr"/>
     </row>
     <row r="11">
-      <c r="A11" t="n">
-        <v>2012</v>
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>2012</t>
+        </is>
       </c>
       <c r="B11" t="n">
         <v>4175</v>
@@ -882,37 +790,21 @@
       <c r="D11" t="n">
         <v>4</v>
       </c>
-      <c r="E11" t="n">
-        <v>0</v>
-      </c>
-      <c r="F11" t="n">
-        <v>0</v>
-      </c>
-      <c r="G11" t="n">
-        <v>0</v>
-      </c>
-      <c r="H11" t="n">
-        <v>0</v>
-      </c>
-      <c r="I11" t="n">
-        <v>0</v>
-      </c>
-      <c r="J11" t="n">
-        <v>0</v>
-      </c>
-      <c r="K11" t="n">
-        <v>0</v>
-      </c>
-      <c r="L11" t="n">
-        <v>0</v>
-      </c>
-      <c r="M11" t="n">
-        <v>0</v>
-      </c>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" t="n">
-        <v>2011</v>
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>2011</t>
+        </is>
       </c>
       <c r="B12" t="n">
         <v>4188</v>
@@ -923,33 +815,19 @@
       <c r="D12" t="n">
         <v>7</v>
       </c>
-      <c r="E12" t="n">
-        <v>0</v>
-      </c>
-      <c r="F12" t="n">
-        <v>0</v>
-      </c>
-      <c r="G12" t="n">
-        <v>0</v>
-      </c>
-      <c r="H12" t="n">
-        <v>0</v>
-      </c>
-      <c r="I12" t="n">
-        <v>0</v>
-      </c>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
       <c r="J12" t="n">
         <v>1</v>
       </c>
-      <c r="K12" t="n">
-        <v>0</v>
-      </c>
+      <c r="K12" t="inlineStr"/>
       <c r="L12" t="n">
         <v>2</v>
       </c>
-      <c r="M12" t="n">
-        <v>0</v>
-      </c>
+      <c r="M12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
added DFs to sheets for export
</commit_message>
<xml_diff>
--- a/BLS_Hourly_Wage/Warehouse_BLS.xlsx
+++ b/BLS_Hourly_Wage/Warehouse_BLS.xlsx
@@ -7,7 +7,19 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="df_merged" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="df_all" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Total fatalities" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Private industrys" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="General warehousing and storage" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Under 16 years" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="16 to 17 years" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="18 to 19 years" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="20 to 24 years" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="25 to 34 years" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="35 to 44 years" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="45 to 54 years" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="55 to 64 years" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="65 years and over" sheetId="13" state="visible" r:id="rId13"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -832,4 +844,1152 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>year</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>General warehousing and storage - 35 to 44 years</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>2014</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>2011</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>year</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>General warehousing and storage - 45 to 54 years</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>2017</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>2016</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>2015</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>2013</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>year</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>General warehousing and storage - 55 to 64 years</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>2016</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>2013</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>2011</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>year</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>General warehousing and storage - 65 years and over</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>2017</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>2014</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>year</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Total fatalities</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>4728</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>4349</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>4907</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>4779</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>2017</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>4674</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>2016</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>4693</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>2015</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>4379</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>2014</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>4386</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>2013</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>4101</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>2012</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>4175</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>2011</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>4188</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>year</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Private industrys</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>4728</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>4349</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>4907</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>4779</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>2017</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>4674</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>2016</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>4693</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>2015</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>4379</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>2014</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>4386</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>2013</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>4101</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>2012</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>4175</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>2011</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>4188</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>year</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>General warehousing and storage</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>2017</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>2016</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>2015</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>2014</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>2013</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>2012</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>2011</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>year</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>General warehousing and storage - Under 16 years</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>2011</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>2012</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2013</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>2014</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>2016</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>2017</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>2018</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>2019</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>year</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>General warehousing and storage - 16 to 17 years</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>2011</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>2012</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2013</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>2014</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>2016</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>2017</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>2018</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>2019</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>year</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>General warehousing and storage - 18 to 19 years</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>2015</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>year</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>General warehousing and storage - 20 to 24 years</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>2016</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>year</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>General warehousing and storage - 25 to 34 years</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>2017</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>2014</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>2013</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
removed set_index, excel index to False
</commit_message>
<xml_diff>
--- a/BLS_Hourly_Wage/Warehouse_BLS.xlsx
+++ b/BLS_Hourly_Wage/Warehouse_BLS.xlsx
@@ -437,7 +437,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M12"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,360 +448,306 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>year</t>
+          <t>Total fatalities</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Total fatalities</t>
+          <t>Private industrys</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Private industrys</t>
+          <t>General warehousing and storage</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>General warehousing and storage</t>
+          <t>General warehousing and storage - Under 16 years</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>General warehousing and storage - Under 16 years</t>
+          <t>General warehousing and storage - 16 to 17 years</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>General warehousing and storage - 16 to 17 years</t>
+          <t>General warehousing and storage - 18 to 19 years</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>General warehousing and storage - 18 to 19 years</t>
+          <t>General warehousing and storage - 20 to 24 years</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>General warehousing and storage - 20 to 24 years</t>
+          <t>General warehousing and storage - 25 to 34 years</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>General warehousing and storage - 25 to 34 years</t>
+          <t>General warehousing and storage - 35 to 44 years</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>General warehousing and storage - 35 to 44 years</t>
+          <t>General warehousing and storage - 45 to 54 years</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>General warehousing and storage - 45 to 54 years</t>
+          <t>General warehousing and storage - 55 to 64 years</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>General warehousing and storage - 55 to 64 years</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
           <t>General warehousing and storage - 65 years and over</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
+      <c r="A2" t="n">
+        <v>4728</v>
       </c>
       <c r="B2" t="n">
         <v>4728</v>
       </c>
       <c r="C2" t="n">
-        <v>4728</v>
-      </c>
-      <c r="D2" t="n">
         <v>36</v>
       </c>
+      <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
+      <c r="H2" t="n">
+        <v>10</v>
+      </c>
       <c r="I2" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="J2" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="K2" t="n">
-        <v>9</v>
-      </c>
-      <c r="L2" t="n">
         <v>7</v>
       </c>
-      <c r="M2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>2020</t>
-        </is>
+      <c r="A3" t="n">
+        <v>4349</v>
       </c>
       <c r="B3" t="n">
         <v>4349</v>
       </c>
       <c r="C3" t="n">
-        <v>4349</v>
-      </c>
-      <c r="D3" t="n">
         <v>11</v>
       </c>
+      <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="n">
+      <c r="G3" t="n">
         <v>1</v>
       </c>
+      <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="n">
+      <c r="K3" t="n">
         <v>3</v>
       </c>
-      <c r="M3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>2019</t>
-        </is>
+      <c r="A4" t="n">
+        <v>4907</v>
       </c>
       <c r="B4" t="n">
         <v>4907</v>
       </c>
       <c r="C4" t="n">
-        <v>4907</v>
-      </c>
-      <c r="D4" t="n">
         <v>17</v>
       </c>
+      <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
+      <c r="J4" t="n">
+        <v>4</v>
+      </c>
       <c r="K4" t="n">
-        <v>4</v>
-      </c>
-      <c r="L4" t="n">
         <v>5</v>
       </c>
-      <c r="M4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
-          <t>2018</t>
-        </is>
+      <c r="A5" t="n">
+        <v>4779</v>
       </c>
       <c r="B5" t="n">
         <v>4779</v>
       </c>
       <c r="C5" t="n">
-        <v>4779</v>
-      </c>
-      <c r="D5" t="n">
         <v>13</v>
       </c>
+      <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="n">
+      <c r="H5" t="n">
         <v>4</v>
       </c>
+      <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
+      <c r="K5" t="n">
+        <v>3</v>
+      </c>
       <c r="L5" t="n">
-        <v>3</v>
-      </c>
-      <c r="M5" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>2017</t>
-        </is>
+      <c r="A6" t="n">
+        <v>4674</v>
       </c>
       <c r="B6" t="n">
         <v>4674</v>
       </c>
       <c r="C6" t="n">
-        <v>4674</v>
-      </c>
-      <c r="D6" t="n">
         <v>15</v>
       </c>
+      <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="n">
+      <c r="H6" t="n">
         <v>4</v>
       </c>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="n">
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="n">
         <v>4</v>
       </c>
-      <c r="L6" t="inlineStr"/>
-      <c r="M6" t="n">
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="inlineStr">
-        <is>
-          <t>2016</t>
-        </is>
+      <c r="A7" t="n">
+        <v>4693</v>
       </c>
       <c r="B7" t="n">
         <v>4693</v>
       </c>
       <c r="C7" t="n">
-        <v>4693</v>
-      </c>
-      <c r="D7" t="n">
         <v>12</v>
       </c>
+      <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="n">
+      <c r="G7" t="n">
         <v>1</v>
       </c>
+      <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
+      <c r="J7" t="n">
+        <v>6</v>
+      </c>
       <c r="K7" t="n">
-        <v>6</v>
-      </c>
-      <c r="L7" t="n">
         <v>4</v>
       </c>
-      <c r="M7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="inlineStr">
-        <is>
-          <t>2015</t>
-        </is>
+      <c r="A8" t="n">
+        <v>4379</v>
       </c>
       <c r="B8" t="n">
         <v>4379</v>
       </c>
       <c r="C8" t="n">
-        <v>4379</v>
-      </c>
-      <c r="D8" t="n">
         <v>6</v>
       </c>
+      <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="n">
+      <c r="F8" t="n">
         <v>1</v>
       </c>
+      <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr"/>
       <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="n">
+      <c r="J8" t="n">
         <v>1</v>
       </c>
+      <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr"/>
-      <c r="M8" t="inlineStr"/>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="inlineStr">
-        <is>
-          <t>2014</t>
-        </is>
+      <c r="A9" t="n">
+        <v>4386</v>
       </c>
       <c r="B9" t="n">
         <v>4386</v>
       </c>
       <c r="C9" t="n">
-        <v>4386</v>
-      </c>
-      <c r="D9" t="n">
         <v>13</v>
       </c>
+      <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
+      <c r="H9" t="n">
+        <v>3</v>
+      </c>
       <c r="I9" t="n">
-        <v>3</v>
-      </c>
-      <c r="J9" t="n">
         <v>1</v>
       </c>
+      <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
-      <c r="M9" t="n">
+      <c r="L9" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="inlineStr">
-        <is>
-          <t>2013</t>
-        </is>
+      <c r="A10" t="n">
+        <v>4101</v>
       </c>
       <c r="B10" t="n">
         <v>4101</v>
       </c>
       <c r="C10" t="n">
-        <v>4101</v>
-      </c>
-      <c r="D10" t="n">
         <v>13</v>
       </c>
+      <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="n">
+      <c r="H10" t="n">
         <v>5</v>
       </c>
-      <c r="J10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="n">
+        <v>3</v>
+      </c>
       <c r="K10" t="n">
         <v>3</v>
       </c>
-      <c r="L10" t="n">
-        <v>3</v>
-      </c>
-      <c r="M10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="inlineStr">
-        <is>
-          <t>2012</t>
-        </is>
+      <c r="A11" t="n">
+        <v>4175</v>
       </c>
       <c r="B11" t="n">
         <v>4175</v>
       </c>
       <c r="C11" t="n">
-        <v>4175</v>
-      </c>
-      <c r="D11" t="n">
         <v>4</v>
       </c>
+      <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr"/>
@@ -810,36 +756,30 @@
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
-      <c r="M11" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="inlineStr">
-        <is>
-          <t>2011</t>
-        </is>
+      <c r="A12" t="n">
+        <v>4188</v>
       </c>
       <c r="B12" t="n">
         <v>4188</v>
       </c>
       <c r="C12" t="n">
-        <v>4188</v>
-      </c>
-      <c r="D12" t="n">
         <v>7</v>
       </c>
+      <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr"/>
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
-      <c r="J12" t="n">
+      <c r="I12" t="n">
         <v>1</v>
       </c>
-      <c r="K12" t="inlineStr"/>
-      <c r="L12" t="n">
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="n">
         <v>2</v>
       </c>
-      <c r="M12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -873,7 +813,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
+      <c r="A2" t="inlineStr">
         <is>
           <t>2021</t>
         </is>
@@ -883,7 +823,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="inlineStr">
+      <c r="A3" t="inlineStr">
         <is>
           <t>2014</t>
         </is>
@@ -893,7 +833,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="inlineStr">
+      <c r="A4" t="inlineStr">
         <is>
           <t>2011</t>
         </is>
@@ -934,7 +874,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
+      <c r="A2" t="inlineStr">
         <is>
           <t>2021</t>
         </is>
@@ -944,7 +884,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="inlineStr">
+      <c r="A3" t="inlineStr">
         <is>
           <t>2019</t>
         </is>
@@ -954,7 +894,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="inlineStr">
+      <c r="A4" t="inlineStr">
         <is>
           <t>2017</t>
         </is>
@@ -964,7 +904,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="inlineStr">
+      <c r="A5" t="inlineStr">
         <is>
           <t>2016</t>
         </is>
@@ -974,7 +914,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="inlineStr">
+      <c r="A6" t="inlineStr">
         <is>
           <t>2015</t>
         </is>
@@ -984,7 +924,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="inlineStr">
+      <c r="A7" t="inlineStr">
         <is>
           <t>2013</t>
         </is>
@@ -1025,7 +965,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
+      <c r="A2" t="inlineStr">
         <is>
           <t>2021</t>
         </is>
@@ -1035,7 +975,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="inlineStr">
+      <c r="A3" t="inlineStr">
         <is>
           <t>2020</t>
         </is>
@@ -1045,7 +985,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="inlineStr">
+      <c r="A4" t="inlineStr">
         <is>
           <t>2019</t>
         </is>
@@ -1055,7 +995,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="inlineStr">
+      <c r="A5" t="inlineStr">
         <is>
           <t>2018</t>
         </is>
@@ -1065,7 +1005,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="inlineStr">
+      <c r="A6" t="inlineStr">
         <is>
           <t>2016</t>
         </is>
@@ -1075,7 +1015,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="inlineStr">
+      <c r="A7" t="inlineStr">
         <is>
           <t>2013</t>
         </is>
@@ -1085,7 +1025,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="inlineStr">
+      <c r="A8" t="inlineStr">
         <is>
           <t>2011</t>
         </is>
@@ -1126,7 +1066,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
+      <c r="A2" t="inlineStr">
         <is>
           <t>2018</t>
         </is>
@@ -1136,7 +1076,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="inlineStr">
+      <c r="A3" t="inlineStr">
         <is>
           <t>2017</t>
         </is>
@@ -1146,7 +1086,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="inlineStr">
+      <c r="A4" t="inlineStr">
         <is>
           <t>2014</t>
         </is>
@@ -1187,7 +1127,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
+      <c r="A2" t="inlineStr">
         <is>
           <t>2021</t>
         </is>
@@ -1197,7 +1137,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="inlineStr">
+      <c r="A3" t="inlineStr">
         <is>
           <t>2020</t>
         </is>
@@ -1207,7 +1147,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="inlineStr">
+      <c r="A4" t="inlineStr">
         <is>
           <t>2019</t>
         </is>
@@ -1217,7 +1157,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="inlineStr">
+      <c r="A5" t="inlineStr">
         <is>
           <t>2018</t>
         </is>
@@ -1227,7 +1167,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="inlineStr">
+      <c r="A6" t="inlineStr">
         <is>
           <t>2017</t>
         </is>
@@ -1237,7 +1177,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="inlineStr">
+      <c r="A7" t="inlineStr">
         <is>
           <t>2016</t>
         </is>
@@ -1247,7 +1187,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="inlineStr">
+      <c r="A8" t="inlineStr">
         <is>
           <t>2015</t>
         </is>
@@ -1257,7 +1197,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="inlineStr">
+      <c r="A9" t="inlineStr">
         <is>
           <t>2014</t>
         </is>
@@ -1267,7 +1207,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="inlineStr">
+      <c r="A10" t="inlineStr">
         <is>
           <t>2013</t>
         </is>
@@ -1277,7 +1217,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="inlineStr">
+      <c r="A11" t="inlineStr">
         <is>
           <t>2012</t>
         </is>
@@ -1287,7 +1227,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="inlineStr">
+      <c r="A12" t="inlineStr">
         <is>
           <t>2011</t>
         </is>
@@ -1328,7 +1268,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
+      <c r="A2" t="inlineStr">
         <is>
           <t>2021</t>
         </is>
@@ -1338,7 +1278,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="inlineStr">
+      <c r="A3" t="inlineStr">
         <is>
           <t>2020</t>
         </is>
@@ -1348,7 +1288,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="inlineStr">
+      <c r="A4" t="inlineStr">
         <is>
           <t>2019</t>
         </is>
@@ -1358,7 +1298,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="inlineStr">
+      <c r="A5" t="inlineStr">
         <is>
           <t>2018</t>
         </is>
@@ -1368,7 +1308,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="inlineStr">
+      <c r="A6" t="inlineStr">
         <is>
           <t>2017</t>
         </is>
@@ -1378,7 +1318,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="inlineStr">
+      <c r="A7" t="inlineStr">
         <is>
           <t>2016</t>
         </is>
@@ -1388,7 +1328,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="inlineStr">
+      <c r="A8" t="inlineStr">
         <is>
           <t>2015</t>
         </is>
@@ -1398,7 +1338,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="inlineStr">
+      <c r="A9" t="inlineStr">
         <is>
           <t>2014</t>
         </is>
@@ -1408,7 +1348,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="inlineStr">
+      <c r="A10" t="inlineStr">
         <is>
           <t>2013</t>
         </is>
@@ -1418,7 +1358,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="inlineStr">
+      <c r="A11" t="inlineStr">
         <is>
           <t>2012</t>
         </is>
@@ -1428,7 +1368,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="inlineStr">
+      <c r="A12" t="inlineStr">
         <is>
           <t>2011</t>
         </is>
@@ -1469,7 +1409,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
+      <c r="A2" t="inlineStr">
         <is>
           <t>2021</t>
         </is>
@@ -1479,7 +1419,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="inlineStr">
+      <c r="A3" t="inlineStr">
         <is>
           <t>2020</t>
         </is>
@@ -1489,7 +1429,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="inlineStr">
+      <c r="A4" t="inlineStr">
         <is>
           <t>2019</t>
         </is>
@@ -1499,7 +1439,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="inlineStr">
+      <c r="A5" t="inlineStr">
         <is>
           <t>2018</t>
         </is>
@@ -1509,7 +1449,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="inlineStr">
+      <c r="A6" t="inlineStr">
         <is>
           <t>2017</t>
         </is>
@@ -1519,7 +1459,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="inlineStr">
+      <c r="A7" t="inlineStr">
         <is>
           <t>2016</t>
         </is>
@@ -1529,7 +1469,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="inlineStr">
+      <c r="A8" t="inlineStr">
         <is>
           <t>2015</t>
         </is>
@@ -1539,7 +1479,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="inlineStr">
+      <c r="A9" t="inlineStr">
         <is>
           <t>2014</t>
         </is>
@@ -1549,7 +1489,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="inlineStr">
+      <c r="A10" t="inlineStr">
         <is>
           <t>2013</t>
         </is>
@@ -1559,7 +1499,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="inlineStr">
+      <c r="A11" t="inlineStr">
         <is>
           <t>2012</t>
         </is>
@@ -1569,7 +1509,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="inlineStr">
+      <c r="A12" t="inlineStr">
         <is>
           <t>2011</t>
         </is>
@@ -1610,7 +1550,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
+      <c r="A2" t="n">
         <v>2011</v>
       </c>
       <c r="B2" t="n">
@@ -1618,7 +1558,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="n">
+      <c r="A3" t="n">
         <v>2012</v>
       </c>
       <c r="B3" t="n">
@@ -1626,7 +1566,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="n">
+      <c r="A4" t="n">
         <v>2013</v>
       </c>
       <c r="B4" t="n">
@@ -1634,7 +1574,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="n">
+      <c r="A5" t="n">
         <v>2014</v>
       </c>
       <c r="B5" t="n">
@@ -1642,7 +1582,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="n">
+      <c r="A6" t="n">
         <v>2015</v>
       </c>
       <c r="B6" t="n">
@@ -1650,7 +1590,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="n">
+      <c r="A7" t="n">
         <v>2016</v>
       </c>
       <c r="B7" t="n">
@@ -1658,7 +1598,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="n">
+      <c r="A8" t="n">
         <v>2017</v>
       </c>
       <c r="B8" t="n">
@@ -1666,7 +1606,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="n">
+      <c r="A9" t="n">
         <v>2018</v>
       </c>
       <c r="B9" t="n">
@@ -1674,7 +1614,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="n">
+      <c r="A10" t="n">
         <v>2019</v>
       </c>
       <c r="B10" t="n">
@@ -1682,7 +1622,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="n">
+      <c r="A11" t="n">
         <v>2020</v>
       </c>
       <c r="B11" t="n">
@@ -1690,7 +1630,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="n">
+      <c r="A12" t="n">
         <v>2021</v>
       </c>
       <c r="B12" t="n">
@@ -1729,7 +1669,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
+      <c r="A2" t="n">
         <v>2011</v>
       </c>
       <c r="B2" t="n">
@@ -1737,7 +1677,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="n">
+      <c r="A3" t="n">
         <v>2012</v>
       </c>
       <c r="B3" t="n">
@@ -1745,7 +1685,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="n">
+      <c r="A4" t="n">
         <v>2013</v>
       </c>
       <c r="B4" t="n">
@@ -1753,7 +1693,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="n">
+      <c r="A5" t="n">
         <v>2014</v>
       </c>
       <c r="B5" t="n">
@@ -1761,7 +1701,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="n">
+      <c r="A6" t="n">
         <v>2015</v>
       </c>
       <c r="B6" t="n">
@@ -1769,7 +1709,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="n">
+      <c r="A7" t="n">
         <v>2016</v>
       </c>
       <c r="B7" t="n">
@@ -1777,7 +1717,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="n">
+      <c r="A8" t="n">
         <v>2017</v>
       </c>
       <c r="B8" t="n">
@@ -1785,7 +1725,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="n">
+      <c r="A9" t="n">
         <v>2018</v>
       </c>
       <c r="B9" t="n">
@@ -1793,7 +1733,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="n">
+      <c r="A10" t="n">
         <v>2019</v>
       </c>
       <c r="B10" t="n">
@@ -1801,7 +1741,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="n">
+      <c r="A11" t="n">
         <v>2020</v>
       </c>
       <c r="B11" t="n">
@@ -1809,7 +1749,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="n">
+      <c r="A12" t="n">
         <v>2021</v>
       </c>
       <c r="B12" t="n">
@@ -1848,7 +1788,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
+      <c r="A2" t="inlineStr">
         <is>
           <t>2015</t>
         </is>
@@ -1889,7 +1829,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
+      <c r="A2" t="inlineStr">
         <is>
           <t>2020</t>
         </is>
@@ -1899,7 +1839,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="inlineStr">
+      <c r="A3" t="inlineStr">
         <is>
           <t>2016</t>
         </is>
@@ -1940,7 +1880,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
+      <c r="A2" t="inlineStr">
         <is>
           <t>2021</t>
         </is>
@@ -1950,7 +1890,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="inlineStr">
+      <c r="A3" t="inlineStr">
         <is>
           <t>2018</t>
         </is>
@@ -1960,7 +1900,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="inlineStr">
+      <c r="A4" t="inlineStr">
         <is>
           <t>2017</t>
         </is>
@@ -1970,7 +1910,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="inlineStr">
+      <c r="A5" t="inlineStr">
         <is>
           <t>2014</t>
         </is>
@@ -1980,7 +1920,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="inlineStr">
+      <c r="A6" t="inlineStr">
         <is>
           <t>2013</t>
         </is>

</xml_diff>

<commit_message>
renamed 'year' to 'Year' in all DF
</commit_message>
<xml_diff>
--- a/BLS_Hourly_Wage/Warehouse_BLS.xlsx
+++ b/BLS_Hourly_Wage/Warehouse_BLS.xlsx
@@ -803,12 +803,12 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>year</t>
+          <t>Year</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>General warehousing and storage - 35 to 44 years</t>
+          <t>General Warehousing and Storage - 35 to 44 Years</t>
         </is>
       </c>
     </row>
@@ -864,12 +864,12 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>year</t>
+          <t>Year</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>General warehousing and storage - 45 to 54 years</t>
+          <t>General Warehousing and Storage - 45 to 54 Years</t>
         </is>
       </c>
     </row>
@@ -955,12 +955,12 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>year</t>
+          <t>Year</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>General warehousing and storage - 55 to 64 years</t>
+          <t>General Warehousing and Storage - 55 to 64 Years</t>
         </is>
       </c>
     </row>
@@ -1056,7 +1056,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>year</t>
+          <t>Year</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -1117,12 +1117,12 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>year</t>
+          <t>Year</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Total fatalities</t>
+          <t>Total Fatalities</t>
         </is>
       </c>
     </row>
@@ -1258,12 +1258,12 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>year</t>
+          <t>Year</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Private industrys</t>
+          <t>Private Industrys</t>
         </is>
       </c>
     </row>
@@ -1399,12 +1399,12 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>year</t>
+          <t>Year</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>General warehousing and storage</t>
+          <t>General Warehousing and Storage</t>
         </is>
       </c>
     </row>
@@ -1540,12 +1540,12 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>year</t>
+          <t>Year</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>General warehousing and storage - Under 16 years</t>
+          <t>General Warehousing and Storage - Under 16 Years</t>
         </is>
       </c>
     </row>
@@ -1659,12 +1659,12 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>year</t>
+          <t>Year</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>General warehousing and storage - 16 to 17 years</t>
+          <t>General Warehousing and Storage - 16 to 17 Years</t>
         </is>
       </c>
     </row>
@@ -1778,12 +1778,12 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>year</t>
+          <t>Year</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>General warehousing and storage - 18 to 19 years</t>
+          <t>General Warehousing and Storage - 18 to 19 Years</t>
         </is>
       </c>
     </row>
@@ -1819,12 +1819,12 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>year</t>
+          <t>Year</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>General warehousing and storage - 20 to 24 years</t>
+          <t>General Warehousing and Storage - 20 to 24 Years</t>
         </is>
       </c>
     </row>
@@ -1870,12 +1870,12 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>year</t>
+          <t>Year</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>General warehousing and storage - 25 to 34 years</t>
+          <t>General Warehousing and Storage - 25 to 34 Years</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
added clustered bar, troubleshooting clustered bar
</commit_message>
<xml_diff>
--- a/BLS_Hourly_Wage/Warehouse_BLS.xlsx
+++ b/BLS_Hourly_Wage/Warehouse_BLS.xlsx
@@ -17,7 +17,7 @@
     <sheet name="20 to 24 Years" sheetId="8" state="visible" r:id="rId8"/>
     <sheet name="25 to 34 Years" sheetId="9" state="visible" r:id="rId9"/>
     <sheet name="35 to 44 Years" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="45 to 94 Years" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="45 to 54 Years" sheetId="11" state="visible" r:id="rId11"/>
     <sheet name="55 to 64 Years" sheetId="12" state="visible" r:id="rId12"/>
     <sheet name="65 Years and Over" sheetId="13" state="visible" r:id="rId13"/>
   </sheets>
@@ -498,7 +498,7 @@
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>General Warehousing &amp; Storage - 45 to 94 Years</t>
+          <t>General Warehousing &amp; Storage - 45 to 54 Years</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
@@ -529,12 +529,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G2" t="n">
@@ -576,12 +576,12 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G3" t="n">
@@ -623,12 +623,12 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G4" t="n">
@@ -670,12 +670,12 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G5" t="n">
@@ -717,12 +717,12 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G6" t="n">
@@ -764,12 +764,12 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G7" t="n">
@@ -811,12 +811,12 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G8" t="n">
@@ -858,12 +858,12 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G9" t="n">
@@ -905,12 +905,12 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G10" t="n">
@@ -952,12 +952,12 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G11" t="n">
@@ -999,12 +999,12 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G12" t="n">
@@ -1197,7 +1197,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>General Warehousing &amp; Storage - 45 to 94 Years</t>
+          <t>General Warehousing &amp; Storage - 45 to 54 Years</t>
         </is>
       </c>
     </row>
@@ -2055,7 +2055,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -2067,7 +2067,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -2079,7 +2079,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -2091,7 +2091,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -2103,7 +2103,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -2115,7 +2115,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -2127,7 +2127,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -2139,7 +2139,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -2151,7 +2151,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -2163,7 +2163,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -2175,7 +2175,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -2218,7 +2218,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -2230,7 +2230,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -2242,7 +2242,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -2254,7 +2254,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -2266,7 +2266,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -2278,7 +2278,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -2290,7 +2290,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -2302,7 +2302,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -2314,7 +2314,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -2326,7 +2326,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -2338,7 +2338,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
corrected dtype in IF statements
</commit_message>
<xml_diff>
--- a/BLS_Hourly_Wage/Warehouse_BLS.xlsx
+++ b/BLS_Hourly_Wage/Warehouse_BLS.xlsx
@@ -527,15 +527,11 @@
       <c r="D2" t="n">
         <v>7</v>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
@@ -574,15 +570,11 @@
       <c r="D3" t="n">
         <v>4</v>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
@@ -621,15 +613,11 @@
       <c r="D4" t="n">
         <v>13</v>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
       </c>
       <c r="G4" t="n">
         <v>0</v>
@@ -668,15 +656,11 @@
       <c r="D5" t="n">
         <v>13</v>
       </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
       </c>
       <c r="G5" t="n">
         <v>0</v>
@@ -715,15 +699,11 @@
       <c r="D6" t="n">
         <v>6</v>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
       </c>
       <c r="G6" t="n">
         <v>1</v>
@@ -762,15 +742,11 @@
       <c r="D7" t="n">
         <v>12</v>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
       </c>
       <c r="G7" t="n">
         <v>0</v>
@@ -809,15 +785,11 @@
       <c r="D8" t="n">
         <v>15</v>
       </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
       </c>
       <c r="G8" t="n">
         <v>0</v>
@@ -856,15 +828,11 @@
       <c r="D9" t="n">
         <v>13</v>
       </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
       </c>
       <c r="G9" t="n">
         <v>0</v>
@@ -903,15 +871,11 @@
       <c r="D10" t="n">
         <v>17</v>
       </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
+      <c r="E10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0</v>
       </c>
       <c r="G10" t="n">
         <v>0</v>
@@ -950,15 +914,11 @@
       <c r="D11" t="n">
         <v>11</v>
       </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
+      <c r="E11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0</v>
       </c>
       <c r="G11" t="n">
         <v>0</v>
@@ -997,15 +957,11 @@
       <c r="D12" t="n">
         <v>36</v>
       </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
+      <c r="E12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0</v>
       </c>
       <c r="G12" t="n">
         <v>0</v>
@@ -2053,10 +2009,8 @@
           <t>2011</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
+      <c r="B2" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -2065,10 +2019,8 @@
           <t>2012</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
+      <c r="B3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -2077,10 +2029,8 @@
           <t>2013</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
+      <c r="B4" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -2089,10 +2039,8 @@
           <t>2014</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
+      <c r="B5" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -2101,10 +2049,8 @@
           <t>2015</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
+      <c r="B6" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -2113,10 +2059,8 @@
           <t>2016</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
+      <c r="B7" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -2125,10 +2069,8 @@
           <t>2017</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
+      <c r="B8" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -2137,10 +2079,8 @@
           <t>2018</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
+      <c r="B9" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -2149,10 +2089,8 @@
           <t>2019</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
+      <c r="B10" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -2161,10 +2099,8 @@
           <t>2020</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
+      <c r="B11" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -2173,10 +2109,8 @@
           <t>2021</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
+      <c r="B12" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2216,10 +2150,8 @@
           <t>2011</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
+      <c r="B2" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -2228,10 +2160,8 @@
           <t>2012</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
+      <c r="B3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -2240,10 +2170,8 @@
           <t>2013</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
+      <c r="B4" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -2252,10 +2180,8 @@
           <t>2014</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
+      <c r="B5" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -2264,10 +2190,8 @@
           <t>2015</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
+      <c r="B6" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -2276,10 +2200,8 @@
           <t>2016</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
+      <c r="B7" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -2288,10 +2210,8 @@
           <t>2017</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
+      <c r="B8" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -2300,10 +2220,8 @@
           <t>2018</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
+      <c r="B9" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -2312,10 +2230,8 @@
           <t>2019</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
+      <c r="B10" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -2324,10 +2240,8 @@
           <t>2020</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
+      <c r="B11" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -2336,10 +2250,8 @@
           <t>2021</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
+      <c r="B12" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
saving charts as .png and exporting to WB sheets
</commit_message>
<xml_diff>
--- a/BLS_Hourly_Wage/Warehouse_BLS.xlsx
+++ b/BLS_Hourly_Wage/Warehouse_BLS.xlsx
@@ -146,6 +146,64 @@
     </indexedColors>
   </colors>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6667500" cy="4762500"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6667500" cy="4762500"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="2" name="Image 2" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -432,7 +490,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -987,6 +1045,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
png and png to excel completed
</commit_message>
<xml_diff>
--- a/BLS_Hourly_Wage/Warehouse_BLS.xlsx
+++ b/BLS_Hourly_Wage/Warehouse_BLS.xlsx
@@ -199,6 +199,514 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6667500" cy="4762500"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="3" name="Image 3" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6667500" cy="4762500"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6667500" cy="4762500"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6667500" cy="4762500"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing13.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6667500" cy="4762500"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6667500" cy="4762500"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6667500" cy="4762500"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="2" name="Image 2" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6667500" cy="4762500"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="3" name="Image 3" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6667500" cy="4762500"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6667500" cy="4762500"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="2" name="Image 2" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6667500" cy="4762500"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6667500" cy="4762500"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6667500" cy="4762500"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6667500" cy="4762500"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6667500" cy="4762500"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6667500" cy="4762500"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -1050,7 +1558,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -1187,11 +1695,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -1328,11 +1837,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -1469,11 +1979,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -1610,11 +2121,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -1751,11 +2263,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -1892,11 +2405,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -2033,11 +2547,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -2174,11 +2689,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -2315,11 +2831,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -2456,11 +2973,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -2597,11 +3115,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -2738,5 +3257,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated fig label and locations
</commit_message>
<xml_diff>
--- a/BLS_Hourly_Wage/Warehouse_BLS.xlsx
+++ b/BLS_Hourly_Wage/Warehouse_BLS.xlsx
@@ -318,6 +318,115 @@
     </pic>
     <clientData/>
   </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6667500" cy="4762500"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="7" name="Image 7" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6667500" cy="4762500"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="8" name="Image 8" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6667500" cy="4762500"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="9" name="Image 9" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6667500" cy="4762500"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="10" name="Image 10" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
 </wsDr>
 </file>
 
@@ -379,6 +488,34 @@
     </pic>
     <clientData/>
   </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6667500" cy="4762500"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="3" name="Image 3" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
 </wsDr>
 </file>
 
@@ -440,6 +577,34 @@
     </pic>
     <clientData/>
   </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6667500" cy="4762500"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="3" name="Image 3" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
 </wsDr>
 </file>
 
@@ -501,6 +666,62 @@
     </pic>
     <clientData/>
   </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6667500" cy="4762500"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="3" name="Image 3" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6667500" cy="4762500"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="4" name="Image 4" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
 </wsDr>
 </file>
 
@@ -646,6 +867,538 @@
     </pic>
     <clientData/>
   </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6667500" cy="4762500"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="6" name="Image 6" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6667500" cy="4762500"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="7" name="Image 7" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6667500" cy="4762500"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="8" name="Image 8" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6667500" cy="4762500"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="9" name="Image 9" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6667500" cy="4762500"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="10" name="Image 10" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6667500" cy="4762500"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="11" name="Image 11" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6667500" cy="4762500"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="12" name="Image 12" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6667500" cy="4762500"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="13" name="Image 13" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6667500" cy="4762500"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="14" name="Image 14" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6667500" cy="4762500"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="15" name="Image 15" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6667500" cy="4762500"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="16" name="Image 16" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId16"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6667500" cy="4762500"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="17" name="Image 17" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId17"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6667500" cy="4762500"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="18" name="Image 18" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId18"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6667500" cy="4762500"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="19" name="Image 19" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId19"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6667500" cy="4762500"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="20" name="Image 20" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId20"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6667500" cy="4762500"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="21" name="Image 21" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId21"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6667500" cy="4762500"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="22" name="Image 22" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId22"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6667500" cy="4762500"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="23" name="Image 23" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId23"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6667500" cy="4762500"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="24" name="Image 24" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId24"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
 </wsDr>
 </file>
 
@@ -756,6 +1509,65 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6667500" cy="4762500"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="5" name="Image 5" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6667500" cy="4762500"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="6" name="Image 6" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -849,6 +1661,62 @@
     </pic>
     <clientData/>
   </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6667500" cy="4762500"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="4" name="Image 4" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6667500" cy="4762500"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="5" name="Image 5" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
 </wsDr>
 </file>
 
@@ -910,6 +1778,62 @@
     </pic>
     <clientData/>
   </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6667500" cy="4762500"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="3" name="Image 3" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6667500" cy="4762500"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="4" name="Image 4" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
 </wsDr>
 </file>
 
@@ -971,6 +1895,34 @@
     </pic>
     <clientData/>
   </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6667500" cy="4762500"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="3" name="Image 3" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
 </wsDr>
 </file>
 
@@ -1032,6 +1984,34 @@
     </pic>
     <clientData/>
   </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6667500" cy="4762500"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="3" name="Image 3" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
 </wsDr>
 </file>
 
@@ -1093,6 +2073,34 @@
     </pic>
     <clientData/>
   </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6667500" cy="4762500"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="3" name="Image 3" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
 </wsDr>
 </file>
 
@@ -1154,6 +2162,34 @@
     </pic>
     <clientData/>
   </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6667500" cy="4762500"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="3" name="Image 3" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
 </wsDr>
 </file>
 
@@ -1202,6 +2238,34 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6667500" cy="4762500"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="3" name="Image 3" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId3"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>

</xml_diff>

<commit_message>
updated project plan to include imports & feature
</commit_message>
<xml_diff>
--- a/BLS_Hourly_Wage/Warehouse_BLS.xlsx
+++ b/BLS_Hourly_Wage/Warehouse_BLS.xlsx
@@ -171,258 +171,6 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
-        <a:ln>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>14</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6667500" cy="4762500"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="2" name="Image 2" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-        <a:ln>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>14</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6667500" cy="4762500"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="3" name="Image 3" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-        <a:ln>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>14</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6667500" cy="4762500"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="4" name="Image 4" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId4"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-        <a:ln>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>14</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6667500" cy="4762500"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="5" name="Image 5" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId5"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-        <a:ln>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>14</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6667500" cy="4762500"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="6" name="Image 6" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId6"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-        <a:ln>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>14</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6667500" cy="4762500"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="7" name="Image 7" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId7"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-        <a:ln>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>14</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6667500" cy="4762500"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="8" name="Image 8" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId8"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-        <a:ln>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>14</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6667500" cy="4762500"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="9" name="Image 9" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId9"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-        <a:ln>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>14</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6667500" cy="4762500"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="10" name="Image 10" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId10"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -447,62 +195,6 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-        <a:ln>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>14</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6667500" cy="4762500"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="2" name="Image 2" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-        <a:ln>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>14</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6667500" cy="4762500"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="3" name="Image 3" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId3"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -549,62 +241,6 @@
     </pic>
     <clientData/>
   </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>14</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6667500" cy="4762500"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="2" name="Image 2" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-        <a:ln>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>14</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6667500" cy="4762500"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="3" name="Image 3" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-        <a:ln>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
 </wsDr>
 </file>
 
@@ -625,90 +261,6 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-        <a:ln>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>14</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6667500" cy="4762500"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="2" name="Image 2" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-        <a:ln>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>14</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6667500" cy="4762500"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="3" name="Image 3" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-        <a:ln>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>14</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6667500" cy="4762500"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="4" name="Image 4" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId4"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -755,650 +307,6 @@
     </pic>
     <clientData/>
   </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>14</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6667500" cy="4762500"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="2" name="Image 2" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-        <a:ln>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>14</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6667500" cy="4762500"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="3" name="Image 3" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-        <a:ln>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>14</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6667500" cy="4762500"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="4" name="Image 4" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId4"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-        <a:ln>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>14</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6667500" cy="4762500"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="5" name="Image 5" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId5"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-        <a:ln>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>14</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6667500" cy="4762500"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="6" name="Image 6" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId6"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-        <a:ln>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>14</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6667500" cy="4762500"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="7" name="Image 7" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId7"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-        <a:ln>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>14</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6667500" cy="4762500"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="8" name="Image 8" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId8"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-        <a:ln>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>14</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6667500" cy="4762500"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="9" name="Image 9" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId9"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-        <a:ln>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>14</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6667500" cy="4762500"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="10" name="Image 10" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId10"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-        <a:ln>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>14</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6667500" cy="4762500"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="11" name="Image 11" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId11"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-        <a:ln>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>14</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6667500" cy="4762500"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="12" name="Image 12" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId12"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-        <a:ln>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>14</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6667500" cy="4762500"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="13" name="Image 13" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId13"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-        <a:ln>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>14</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6667500" cy="4762500"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="14" name="Image 14" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId14"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-        <a:ln>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>14</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6667500" cy="4762500"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="15" name="Image 15" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId15"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-        <a:ln>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>14</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6667500" cy="4762500"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="16" name="Image 16" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId16"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-        <a:ln>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>14</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6667500" cy="4762500"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="17" name="Image 17" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId17"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-        <a:ln>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>14</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6667500" cy="4762500"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="18" name="Image 18" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId18"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-        <a:ln>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>14</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6667500" cy="4762500"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="19" name="Image 19" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId19"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-        <a:ln>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>14</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6667500" cy="4762500"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="20" name="Image 20" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId20"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-        <a:ln>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>14</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6667500" cy="4762500"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="21" name="Image 21" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId21"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-        <a:ln>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>14</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6667500" cy="4762500"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="22" name="Image 22" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId22"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-        <a:ln>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>14</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6667500" cy="4762500"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="23" name="Image 23" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId23"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-        <a:ln>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>14</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6667500" cy="4762500"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="24" name="Image 24" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId24"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-        <a:ln>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
 </wsDr>
 </file>
 
@@ -1419,146 +327,6 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-        <a:ln>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>14</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6667500" cy="4762500"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="2" name="Image 2" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-        <a:ln>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>14</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6667500" cy="4762500"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="3" name="Image 3" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-        <a:ln>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>14</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6667500" cy="4762500"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="4" name="Image 4" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId4"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-        <a:ln>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>14</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6667500" cy="4762500"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="5" name="Image 5" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId5"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-        <a:ln>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>14</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6667500" cy="4762500"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="6" name="Image 6" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId6"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1605,118 +373,6 @@
     </pic>
     <clientData/>
   </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>14</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6667500" cy="4762500"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="2" name="Image 2" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-        <a:ln>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>14</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6667500" cy="4762500"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="3" name="Image 3" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-        <a:ln>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>14</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6667500" cy="4762500"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="4" name="Image 4" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId4"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-        <a:ln>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>14</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6667500" cy="4762500"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="5" name="Image 5" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId5"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-        <a:ln>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
 </wsDr>
 </file>
 
@@ -1737,90 +393,6 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-        <a:ln>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>14</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6667500" cy="4762500"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="2" name="Image 2" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-        <a:ln>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>14</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6667500" cy="4762500"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="3" name="Image 3" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-        <a:ln>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>14</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6667500" cy="4762500"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="4" name="Image 4" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId4"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1867,62 +439,6 @@
     </pic>
     <clientData/>
   </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>14</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6667500" cy="4762500"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="2" name="Image 2" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-        <a:ln>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>14</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6667500" cy="4762500"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="3" name="Image 3" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-        <a:ln>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
 </wsDr>
 </file>
 
@@ -1943,62 +459,6 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-        <a:ln>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>14</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6667500" cy="4762500"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="2" name="Image 2" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-        <a:ln>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>14</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6667500" cy="4762500"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="3" name="Image 3" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId3"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2045,62 +505,6 @@
     </pic>
     <clientData/>
   </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>14</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6667500" cy="4762500"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="2" name="Image 2" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-        <a:ln>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>14</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6667500" cy="4762500"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="3" name="Image 3" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-        <a:ln>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
 </wsDr>
 </file>
 
@@ -2134,62 +538,6 @@
     </pic>
     <clientData/>
   </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>14</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6667500" cy="4762500"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="2" name="Image 2" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-        <a:ln>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>14</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6667500" cy="4762500"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="3" name="Image 3" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-        <a:ln>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
 </wsDr>
 </file>
 
@@ -2210,62 +558,6 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-        <a:ln>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>14</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6667500" cy="4762500"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="2" name="Image 2" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-        <a:ln>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>14</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="6667500" cy="4762500"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="3" name="Image 3" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId3"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>

</xml_diff>